<commit_message>
M0a with calibration data
</commit_message>
<xml_diff>
--- a/projects/m0a.xlsx
+++ b/projects/m0a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="14880" windowHeight="7428" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="14880" windowHeight="7428" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -6911,7 +6911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -7342,7 +7342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y130"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
@@ -7499,7 +7499,7 @@
     </row>
     <row r="4" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>869</v>
@@ -7590,7 +7590,7 @@
     </row>
     <row r="9" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>883</v>

</xml_diff>